<commit_message>
patch(epic_questions.py): Increased title length to allow for longer questions
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/evolutionquestions.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/evolutionquestions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9470C1-95D5-4EE6-B83C-6C157E116675}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182594DC-73BE-49EB-B564-AA87957F38FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10545" yWindow="2325" windowWidth="16800" windowHeight="11325" xr2:uid="{5BB4FAED-16CA-424D-B55C-921D539CF78A}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5BB4FAED-16CA-424D-B55C-921D539CF78A}"/>
   </bookViews>
   <sheets>
     <sheet name="evolutionquestions" sheetId="1" r:id="rId1"/>
@@ -425,9 +425,6 @@
     <t xml:space="preserve">WaMOs functioning effectively and are key partners for natural resources and agriculture agencies. Comprehensive watershed plans formulated with broad engagement by other agencies and stakeholders. Watershed plans synergize with river basin plans. </t>
   </si>
   <si>
-    <t>Watershed Planning</t>
-  </si>
-  <si>
     <t>Water Resources Infrastructure</t>
   </si>
   <si>
@@ -777,6 +774,9 @@
   </si>
   <si>
     <t>Overarching Flood Risk Management Framework</t>
+  </si>
+  <si>
+    <t>Watershed Management</t>
   </si>
 </sst>
 </file>
@@ -1230,21 +1230,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD25"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="127.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="108.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="228.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="127.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="228.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,12 +1267,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>13</v>
@@ -1315,12 +1315,12 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>18</v>
@@ -1339,12 +1339,12 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>23</v>
@@ -1363,12 +1363,12 @@
       </c>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>13</v>
@@ -1387,12 +1387,12 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>32</v>
@@ -1411,12 +1411,12 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -1435,12 +1435,12 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>18</v>
@@ -1459,12 +1459,12 @@
       </c>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>2</v>
@@ -1483,12 +1483,12 @@
       </c>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>8</v>
@@ -1507,12 +1507,12 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>13</v>
@@ -1531,12 +1531,12 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>18</v>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>48</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>48</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>48</v>
       </c>
@@ -1603,7 +1603,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>48</v>
       </c>
@@ -1619,7 +1619,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>48</v>
       </c>
@@ -1635,7 +1635,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>48</v>
       </c>
@@ -1651,7 +1651,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>56</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>59</v>
       </c>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>59</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>59</v>
       </c>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>59</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>85</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>85</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>85</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>85</v>
       </c>
@@ -1860,12 +1860,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>106</v>
+      <c r="B30" t="s">
+        <v>188</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6" t="s">
@@ -1881,159 +1881,159 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G31" s="6" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G32" s="6" t="s">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="G33" s="6" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G34" s="6" t="s">
+    </row>
+    <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="G35" s="8" t="s">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G36" s="6" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="G37" s="6" t="s">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6" t="s">
@@ -2049,159 +2049,159 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="G39" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G39" s="6" t="s">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G40" s="6" t="s">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G41" s="6" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="G42" s="6" t="s">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="G43" s="6" t="s">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="G44" s="6" t="s">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>177</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="F45" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="G45" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G45" s="6" t="s">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
+      <c r="B46" s="17" t="s">
         <v>182</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>183</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>50</v>
@@ -2211,12 +2211,12 @@
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>50</v>
@@ -2233,15 +2233,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FD03EABF3F2FB448DAE5CD2CE5D353B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="98b843f414b1d31b21b2b135980a1ce8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be3c9163-79a1-42b6-a061-0833e6c3add8" xmlns:ns4="4e51305d-5de6-45a6-8f4b-ddcbc1e897ba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed93da940882836d4864d93d9a5709d2" ns3:_="" ns4:_="">
     <xsd:import namespace="be3c9163-79a1-42b6-a061-0833e6c3add8"/>
@@ -2470,6 +2461,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2477,14 +2477,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1622E4D1-EB36-4F19-983B-15F91DDCA2CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F90CD483-4F3F-4DF6-9268-711E23AAE775}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2503,6 +2495,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1622E4D1-EB36-4F19-983B-15F91DDCA2CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F4BF107-D120-446E-AB03-5D44E6F3B9B6}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
patch(epic_questions.py): Increased title length to allow for longer … (#74)
* patch(epic_questions.py): Increased title length to allow for longer questions

* docs: Updated key agency actions questions xlsx and related test
</commit_message>
<xml_diff>
--- a/backend/epic_app/tests/test_data/xlsx/evolutionquestions.xlsx
+++ b/backend/epic_app/tests/test_data/xlsx/evolutionquestions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9470C1-95D5-4EE6-B83C-6C157E116675}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182594DC-73BE-49EB-B564-AA87957F38FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10545" yWindow="2325" windowWidth="16800" windowHeight="11325" xr2:uid="{5BB4FAED-16CA-424D-B55C-921D539CF78A}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5BB4FAED-16CA-424D-B55C-921D539CF78A}"/>
   </bookViews>
   <sheets>
     <sheet name="evolutionquestions" sheetId="1" r:id="rId1"/>
@@ -425,9 +425,6 @@
     <t xml:space="preserve">WaMOs functioning effectively and are key partners for natural resources and agriculture agencies. Comprehensive watershed plans formulated with broad engagement by other agencies and stakeholders. Watershed plans synergize with river basin plans. </t>
   </si>
   <si>
-    <t>Watershed Planning</t>
-  </si>
-  <si>
     <t>Water Resources Infrastructure</t>
   </si>
   <si>
@@ -777,6 +774,9 @@
   </si>
   <si>
     <t>Overarching Flood Risk Management Framework</t>
+  </si>
+  <si>
+    <t>Watershed Management</t>
   </si>
 </sst>
 </file>
@@ -1230,21 +1230,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD25"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="127.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="108.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="228.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="127.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="228.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,12 +1267,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>13</v>
@@ -1315,12 +1315,12 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>18</v>
@@ -1339,12 +1339,12 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>23</v>
@@ -1363,12 +1363,12 @@
       </c>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>13</v>
@@ -1387,12 +1387,12 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>32</v>
@@ -1411,12 +1411,12 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -1435,12 +1435,12 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>18</v>
@@ -1459,12 +1459,12 @@
       </c>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>2</v>
@@ -1483,12 +1483,12 @@
       </c>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>8</v>
@@ -1507,12 +1507,12 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>13</v>
@@ -1531,12 +1531,12 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>18</v>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>48</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>48</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>48</v>
       </c>
@@ -1603,7 +1603,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>48</v>
       </c>
@@ -1619,7 +1619,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>48</v>
       </c>
@@ -1635,7 +1635,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>48</v>
       </c>
@@ -1651,7 +1651,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>56</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>59</v>
       </c>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>59</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>59</v>
       </c>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>59</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>85</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>85</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>85</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>85</v>
       </c>
@@ -1860,12 +1860,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>106</v>
+      <c r="B30" t="s">
+        <v>188</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6" t="s">
@@ -1881,159 +1881,159 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G31" s="6" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G32" s="6" t="s">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="G33" s="6" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G34" s="6" t="s">
+    </row>
+    <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="G35" s="8" t="s">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G36" s="6" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="G37" s="6" t="s">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6" t="s">
@@ -2049,159 +2049,159 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="G39" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G39" s="6" t="s">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G40" s="6" t="s">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G41" s="6" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="G42" s="6" t="s">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="G43" s="6" t="s">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="G44" s="6" t="s">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>177</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="F45" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="G45" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G45" s="6" t="s">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
+      <c r="B46" s="17" t="s">
         <v>182</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>183</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>50</v>
@@ -2211,12 +2211,12 @@
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>50</v>
@@ -2233,15 +2233,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FD03EABF3F2FB448DAE5CD2CE5D353B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="98b843f414b1d31b21b2b135980a1ce8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be3c9163-79a1-42b6-a061-0833e6c3add8" xmlns:ns4="4e51305d-5de6-45a6-8f4b-ddcbc1e897ba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed93da940882836d4864d93d9a5709d2" ns3:_="" ns4:_="">
     <xsd:import namespace="be3c9163-79a1-42b6-a061-0833e6c3add8"/>
@@ -2470,6 +2461,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2477,14 +2477,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1622E4D1-EB36-4F19-983B-15F91DDCA2CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F90CD483-4F3F-4DF6-9268-711E23AAE775}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2503,6 +2495,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1622E4D1-EB36-4F19-983B-15F91DDCA2CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F4BF107-D120-446E-AB03-5D44E6F3B9B6}">
   <ds:schemaRefs>

</xml_diff>